<commit_message>
Works in samples(in progress...), fix errors in minicharts, add new attributes in minicharts(Minichart->Size, Minichart>Location>ByRow|ByColumn|Relative|Coordinates (Only ByColumn works!!)). Solved many little errors
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample04-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample04-from-config-file.xlsx
@@ -180,10 +180,10 @@
     <xf numFmtId="164" fontId="3" fillId="5" borderId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -222,10 +222,10 @@
     <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="1" applyBorder="1" xfId="11" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" xfId="12" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="1" applyBorder="1" xfId="13" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" xfId="12" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="1" applyBorder="1" xfId="13" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -280,6 +280,29 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
+            <c:v>Purchase Price</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart And Secondary Axis'!B2:B6</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart And Secondary Axis'!D2:D6</c:f>
+            </c:numRef>
+          </c:val>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="336ea9"/>
+            </a:solidFill>
+          </c:spPr>
+        </ser>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
             <c:v>Profit</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
@@ -296,29 +319,6 @@
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="ed7d31"/>
-            </a:solidFill>
-          </c:spPr>
-        </ser>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Purchase Price</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chart And Secondary Axis'!B2:B6</c:f>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chart And Secondary Axis'!D2:D6</c:f>
-            </c:numRef>
-          </c:val>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="336ea9"/>
             </a:solidFill>
           </c:spPr>
         </ser>
@@ -340,7 +340,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Chart And Secondary Axis'!B2:B6</c:f>
+              <c:f>'Chart And Secondary Axis'!A2:A6</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
@@ -478,7 +478,7 @@
         </c:title>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="low"/>
+        <c:tickLblPos val="high"/>
         <c:crossAx val="4"/>
         <c:txPr>
           <a:bodyPr rot="0" vert="horz"/>
@@ -504,6 +504,7 @@
         <c:axId val="4"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -524,7 +525,7 @@
         </c:title>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="low"/>
+        <c:tickLblPos val="high"/>
         <c:crossAx val="3"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>

</xml_diff>